<commit_message>
Fix unchanged hardcoded year
</commit_message>
<xml_diff>
--- a/penyata-akhir-2023/form2/2LUHUR-2023.xlsx
+++ b/penyata-akhir-2023/form2/2LUHUR-2023.xlsx
@@ -31,7 +31,7 @@
     <t>To :</t>
   </si>
   <si>
-    <t>HOMEROOM 2LUHUR 2022</t>
+    <t>HOMEROOM 2LUHUR 2023</t>
   </si>
   <si>
     <t>MAKTAB RENDAH SAINS MARA GEMENCHEH</t>
@@ -704,10 +704,10 @@
         <v>14</v>
       </c>
       <c r="D16" s="22">
-        <v>3150</v>
+        <v>3200</v>
       </c>
       <c r="E16" s="23">
-        <v>600</v>
+        <v>150</v>
       </c>
       <c r="F16" s="18"/>
       <c r="G16" s="6"/>
@@ -719,10 +719,10 @@
         <v>15</v>
       </c>
       <c r="D17" s="22">
-        <v>4630</v>
+        <v>5670</v>
       </c>
       <c r="E17" s="18">
-        <v>1000</v>
+        <v>710</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="6"/>
@@ -975,7 +975,7 @@
         <v>23</v>
       </c>
       <c r="D36" s="22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E36" s="18">
         <v>0</v>

</xml_diff>